<commit_message>
Comment testing done using mouse tracker
</commit_message>
<xml_diff>
--- a/docs/iTraceTesting.xlsx
+++ b/docs/iTraceTesting.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="issue69" sheetId="1" r:id="rId1"/>
     <sheet name="issue2" sheetId="2" r:id="rId2"/>
+    <sheet name="issue46" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
   <si>
     <t>Trial</t>
   </si>
@@ -101,12 +102,54 @@
   </si>
   <si>
     <t>Extended tracking on project explorer, no PEE to export. Check for correct bounds.</t>
+  </si>
+  <si>
+    <t>all files with all comment types tracked in the same session</t>
+  </si>
+  <si>
+    <t>java file with /**/ comment type, single line, multi-line, space and no space before starting comment</t>
+  </si>
+  <si>
+    <t>java file with // comment type, with and without space before comment, used on side and before method</t>
+  </si>
+  <si>
+    <t>java file with /** \newline */ comment type, with and without space, and /** */ without newline with and without space, no stars on newline with and without space</t>
+  </si>
+  <si>
+    <t>java file with doc comment type /************  *************/ with and without space, doc comment with asterick newline with and without space</t>
+  </si>
+  <si>
+    <t>java file with comment nesting: /* words \newline // words \newline */ with space and no space on the nested single line comment</t>
+  </si>
+  <si>
+    <t>java file with comment nesting // /* words \newline // words \newline // words */, with and withous space, also single line comment with nested asterick single line comment with and without space</t>
+  </si>
+  <si>
+    <t>Captured all variations correctly in JSON and XML. How is a block_comment for all variations.</t>
+  </si>
+  <si>
+    <t>Captured all variations correctly in JSON and XML. How is a doc_comment for all variations.</t>
+  </si>
+  <si>
+    <t>Captured all variations correctly in JSON and XML. How is a line_comment for all variations.</t>
+  </si>
+  <si>
+    <t>Captured correctly in JSON and XML. How is a block_comment.</t>
+  </si>
+  <si>
+    <t>Captured all variations in JSON and XML. Treats all comments in this type of nesting as single line comments. How is a line_comment for all variations.</t>
+  </si>
+  <si>
+    <t>Captured all comment types correctly in JSON and XML.</t>
+  </si>
+  <si>
+    <t>Add tests for cold folding (coming soon)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -124,7 +167,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -149,6 +192,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -162,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -194,6 +243,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -507,7 +559,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -517,18 +569,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.06640625" customWidth="1"/>
-    <col min="5" max="5" width="23.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -539,7 +591,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -554,7 +606,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -569,7 +621,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -584,7 +636,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -639,7 +691,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="6">
         <v>1</v>
       </c>
@@ -647,7 +699,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="6">
         <v>2</v>
       </c>
@@ -655,7 +707,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" s="6">
         <v>3</v>
       </c>
@@ -663,7 +715,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" s="6">
         <v>4</v>
       </c>
@@ -671,7 +723,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="6">
         <v>5</v>
       </c>
@@ -717,14 +769,14 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.73046875" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="6" max="6" width="23.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -800,12 +852,12 @@
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -837,7 +889,7 @@
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <v>4</v>
       </c>
@@ -846,22 +898,22 @@
       </c>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -870,4 +922,185 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>2</v>
+      </c>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>3</v>
+      </c>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>4</v>
+      </c>
+      <c r="B15" s="12"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>5</v>
+      </c>
+      <c r="B16" s="12"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>7</v>
+      </c>
+      <c r="B18" s="12"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>8</v>
+      </c>
+      <c r="B19" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finished code folding testing, test file to come
</commit_message>
<xml_diff>
--- a/docs/iTraceTesting.xlsx
+++ b/docs/iTraceTesting.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="63">
   <si>
     <t>Trial</t>
   </si>
@@ -143,7 +143,73 @@
     <t>Captured all comment types correctly in JSON and XML.</t>
   </si>
   <si>
-    <t>Add tests for cold folding (coming soon)</t>
+    <t>all comment types in one file, tracked</t>
+  </si>
+  <si>
+    <t>code fold one thing (lines 3-61), before start tracking</t>
+  </si>
+  <si>
+    <t>code fold three things (lines 3-61, 95-97, 115-172), before start tracking, not nested things</t>
+  </si>
+  <si>
+    <t>line numbers match AOI being tracked, code that is folded is not tracked, except for the first line</t>
+  </si>
+  <si>
+    <t>code fold one thing (lines 3-61), during tracking</t>
+  </si>
+  <si>
+    <t>code fold three things (lines 3-61, 95-97, 115-172), during tracking, not nested</t>
+  </si>
+  <si>
+    <t>code fold three things (lines 189-194, 175-201, 375-385), before start tracking, nested</t>
+  </si>
+  <si>
+    <t>code fold three things (lines 189-194, 175-201, 375-385), during tracking, nested</t>
+  </si>
+  <si>
+    <t>code fold one thing (lines 3-61), during tracking, unfold it also during tracking</t>
+  </si>
+  <si>
+    <t>code fold two things (95-97, 115-172), during tracking, unfold them also during tracking, not nested</t>
+  </si>
+  <si>
+    <t>code fold three things (lines 189-194, 175-201, 375-385), during tracking, unfold them also during tracking, nested</t>
+  </si>
+  <si>
+    <t>code fold two things (lines 189-194, 175-201), before tracking, unfold them also during tracking, nested</t>
+  </si>
+  <si>
+    <t>code fold two things (95-97, 115-172), before tracking, unfold them also during tracking, not nested</t>
+  </si>
+  <si>
+    <t>for variable declarations across multiple lines that look like Type variablename = …. Tracking doesn't happen in that line until the column where the variable name starts, but will track in the next line starting at column 0 (and further lines), in general for all variable declarations in the first line tracking doesn't start until reaching the variable name column</t>
+  </si>
+  <si>
+    <t>line numbers match AOI being tracked, code that is folded is not tracked, except for the first line, anonymous functions not tracked in code folding and not code folding, considered as part of method it is argument of, comments in anonymous functions are tracked</t>
+  </si>
+  <si>
+    <t>code fold across two files, one on each, before tracking, (lines 115-172 ControlView.java, lines 36-43 Activator.java), ControlView first</t>
+  </si>
+  <si>
+    <t>code fold across two files, one on each, during tracking, (lines 115-172 ControlView.java, lines 36-43 Activator.java), ControlView first</t>
+  </si>
+  <si>
+    <t>code fold across two files, one on each, before tracking, unfold each during tracking, (lines 115-172 ControlView.java, lines 36-43 Activator.java), ControlView first</t>
+  </si>
+  <si>
+    <t>code fold across two files, one on each, during tracking, unfold each during tracking, (lines 115-172 ControlView.java, lines 36-43 Activator.java), folded and unfolded on first file then moved to second file, ControlView first</t>
+  </si>
+  <si>
+    <t>Do while loops aren't tracked</t>
+  </si>
+  <si>
+    <t>same can be said for methods (but not true for where tracking starts on the first line for methods - needs looked into) and comments, @Override is the start line to methods that are overrides</t>
+  </si>
+  <si>
+    <t>Trials 9-19 use ControlView.java from iTrace for testing in issue46 branch</t>
+  </si>
+  <si>
+    <t>Trials 20-23 use ControlView.java and Activator.java from iTrace for testing in issue46 branch</t>
   </si>
 </sst>
 </file>
@@ -211,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -245,8 +311,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -926,10 +993,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,9 +1005,10 @@
     <col min="2" max="2" width="43.7109375" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
     <col min="4" max="4" width="5.85546875" customWidth="1"/>
+    <col min="6" max="6" width="64.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -951,7 +1019,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -966,7 +1034,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -981,7 +1049,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -996,7 +1064,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1007,7 +1075,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1018,7 +1086,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1029,7 +1097,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1040,65 +1108,249 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+      <c r="C9" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="12"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
         <v>1</v>
       </c>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
         <v>2</v>
       </c>
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
         <v>3</v>
       </c>
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
         <v>4</v>
       </c>
-      <c r="B15" s="12"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
+      <c r="B30" s="12"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
         <v>5</v>
       </c>
-      <c r="B16" s="12"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+      <c r="B31" s="12"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
         <v>6</v>
       </c>
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
         <v>7</v>
       </c>
-      <c r="B18" s="12"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
+      <c r="B33" s="12"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
         <v>8</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B34" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>